<commit_message>
Modified the uploaded files
Fixed a bug on mosel Model (sets used as an arrays)
Added some checks
The data for Nadistrasse yield a feasible solution, now.
</commit_message>
<xml_diff>
--- a/school_data_nadistrasse.xlsx
+++ b/school_data_nadistrasse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ambro\Documents\TUM\FallStudie\Xpress_Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ambro\Desktop\ZeitplanProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469F29F8-1F00-43FB-B219-B833FB12208F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231DF057-2F8D-4F70-A4F5-CED5547D7887}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" tabRatio="819" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,12 +23,12 @@
     <sheet name="Lehrerverfügbarkeiten" sheetId="8" r:id="rId8"/>
     <sheet name="Gleichzeitige Fächer" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="218">
   <si>
     <t>Lehrpläne der Klassen pro Woche</t>
   </si>
@@ -651,12 +651,6 @@
     <t>Wag,Glo, Lan, Zed, Kai</t>
   </si>
   <si>
-    <t>Wag ,Glo, Lan, Zed, Kai</t>
-  </si>
-  <si>
-    <t>Wag, Glo, Lan, Zed, Kai</t>
-  </si>
-  <si>
     <t>Wag, Glo, Lan, Kai</t>
   </si>
   <si>
@@ -685,6 +679,9 @@
   </si>
   <si>
     <t>GU, Englisch, Musik, Kunst, Ethik, Studierzeit, Mathe, Deutsch, HSU, HSU_2, Sport, Förderunterricht, Mittagspause, Wahlfach</t>
+  </si>
+  <si>
+    <t>Wag ,Glo, Lan, Kai</t>
   </si>
 </sst>
 </file>
@@ -770,7 +767,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -883,6 +880,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -1057,7 +1066,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1257,6 +1266,23 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1286,17 +1312,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1396,7 +1411,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>467280</xdr:colOff>
+      <xdr:colOff>467279</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
@@ -2353,8 +2368,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42:F43"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2366,18 +2381,18 @@
     <col min="5" max="5" width="5.59765625"/>
     <col min="6" max="6" width="15.59765625" style="2"/>
     <col min="7" max="7" width="23.69921875" style="2"/>
-    <col min="8" max="8" width="8.8984375" style="2"/>
+    <col min="8" max="8" width="25" style="2" customWidth="1"/>
     <col min="9" max="9" width="16.69921875" style="2"/>
     <col min="10" max="1025" width="10.69921875"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
+      <c r="A2" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2578,14 +2593,14 @@
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="101">
-        <v>1</v>
-      </c>
-      <c r="D13" s="102">
-        <v>1</v>
-      </c>
-      <c r="E13" s="102"/>
-      <c r="F13" s="103">
+      <c r="C13" s="90">
+        <v>1</v>
+      </c>
+      <c r="D13" s="91">
+        <v>1</v>
+      </c>
+      <c r="E13" s="91"/>
+      <c r="F13" s="92">
         <v>1</v>
       </c>
       <c r="G13" s="2">
@@ -2700,14 +2715,14 @@
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="101">
-        <v>1</v>
-      </c>
-      <c r="D19" s="102">
-        <v>1</v>
-      </c>
-      <c r="E19" s="102"/>
-      <c r="F19" s="103">
+      <c r="C19" s="90">
+        <v>1</v>
+      </c>
+      <c r="D19" s="91">
+        <v>1</v>
+      </c>
+      <c r="E19" s="91"/>
+      <c r="F19" s="92">
         <v>1</v>
       </c>
       <c r="G19" s="2">
@@ -2821,14 +2836,14 @@
       <c r="B25" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="101">
-        <v>1</v>
-      </c>
-      <c r="D25" s="102">
-        <v>1</v>
-      </c>
-      <c r="E25" s="102"/>
-      <c r="F25" s="103">
+      <c r="C25" s="90">
+        <v>1</v>
+      </c>
+      <c r="D25" s="91">
+        <v>1</v>
+      </c>
+      <c r="E25" s="91"/>
+      <c r="F25" s="92">
         <v>1</v>
       </c>
       <c r="G25" s="2">
@@ -2943,14 +2958,14 @@
       <c r="B31" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="101">
-        <v>1</v>
-      </c>
-      <c r="D31" s="102">
-        <v>1</v>
-      </c>
-      <c r="E31" s="102"/>
-      <c r="F31" s="103">
+      <c r="C31" s="90">
+        <v>1</v>
+      </c>
+      <c r="D31" s="91">
+        <v>1</v>
+      </c>
+      <c r="E31" s="91"/>
+      <c r="F31" s="92">
         <v>1</v>
       </c>
       <c r="G31" s="2">
@@ -3064,14 +3079,14 @@
       <c r="B37" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="101">
-        <v>1</v>
-      </c>
-      <c r="D37" s="102">
-        <v>1</v>
-      </c>
-      <c r="E37" s="102"/>
-      <c r="F37" s="103">
+      <c r="C37" s="90">
+        <v>1</v>
+      </c>
+      <c r="D37" s="91">
+        <v>1</v>
+      </c>
+      <c r="E37" s="91"/>
+      <c r="F37" s="92">
         <v>1</v>
       </c>
       <c r="G37" s="2">
@@ -3232,14 +3247,14 @@
       <c r="B46" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="101">
-        <v>1</v>
-      </c>
-      <c r="D46" s="102">
-        <v>1</v>
-      </c>
-      <c r="E46" s="102"/>
-      <c r="F46" s="103">
+      <c r="C46" s="90">
+        <v>1</v>
+      </c>
+      <c r="D46" s="91">
+        <v>1</v>
+      </c>
+      <c r="E46" s="91"/>
+      <c r="F46" s="92">
         <v>1</v>
       </c>
       <c r="G46" s="2">
@@ -3286,8 +3301,11 @@
       <c r="D48">
         <v>1</v>
       </c>
-      <c r="G48" s="2">
-        <v>1</v>
+      <c r="G48" s="92">
+        <v>2</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3446,17 +3464,17 @@
       <c r="B57" t="s">
         <v>34</v>
       </c>
-      <c r="C57" s="101">
-        <v>2</v>
-      </c>
-      <c r="D57" s="102">
-        <v>0</v>
-      </c>
-      <c r="E57" s="102"/>
-      <c r="F57" s="103">
-        <v>2</v>
-      </c>
-      <c r="G57" s="103">
+      <c r="C57" s="90">
+        <v>2</v>
+      </c>
+      <c r="D57" s="91">
+        <v>0</v>
+      </c>
+      <c r="E57" s="91"/>
+      <c r="F57" s="92">
+        <v>2</v>
+      </c>
+      <c r="G57" s="92">
         <v>1</v>
       </c>
       <c r="H57" s="2"/>
@@ -3464,19 +3482,19 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C58" s="101">
-        <v>1</v>
-      </c>
-      <c r="D58" s="102">
-        <v>1</v>
-      </c>
-      <c r="E58" s="102"/>
-      <c r="F58" s="103">
-        <v>1</v>
-      </c>
-      <c r="G58" s="103">
+        <v>208</v>
+      </c>
+      <c r="C58" s="90">
+        <v>1</v>
+      </c>
+      <c r="D58" s="91">
+        <v>1</v>
+      </c>
+      <c r="E58" s="91"/>
+      <c r="F58" s="92">
+        <v>1</v>
+      </c>
+      <c r="G58" s="92">
         <v>1</v>
       </c>
     </row>
@@ -3541,7 +3559,7 @@
       <c r="F62" s="2">
         <v>2</v>
       </c>
-      <c r="G62" s="103">
+      <c r="G62" s="92">
         <v>2</v>
       </c>
     </row>
@@ -3645,8 +3663,8 @@
       <c r="D67">
         <v>6</v>
       </c>
-      <c r="G67" s="2">
-        <v>1</v>
+      <c r="G67" s="92">
+        <v>2</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>13</v>
@@ -3662,8 +3680,8 @@
       <c r="D68">
         <v>4</v>
       </c>
-      <c r="G68" s="2">
-        <v>1</v>
+      <c r="G68" s="92">
+        <v>2</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>13</v>
@@ -3688,17 +3706,17 @@
       <c r="B70" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C70" s="101">
-        <v>2</v>
-      </c>
-      <c r="D70" s="102">
-        <v>0</v>
-      </c>
-      <c r="E70" s="102"/>
-      <c r="F70" s="103">
-        <v>2</v>
-      </c>
-      <c r="G70" s="103">
+      <c r="C70" s="90">
+        <v>2</v>
+      </c>
+      <c r="D70" s="91">
+        <v>0</v>
+      </c>
+      <c r="E70" s="91"/>
+      <c r="F70" s="92">
+        <v>2</v>
+      </c>
+      <c r="G70" s="92">
         <v>1</v>
       </c>
       <c r="H70" s="2"/>
@@ -3706,19 +3724,19 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B71" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C71" s="101">
-        <v>1</v>
-      </c>
-      <c r="D71" s="102">
-        <v>1</v>
-      </c>
-      <c r="E71" s="102"/>
-      <c r="F71" s="103">
-        <v>1</v>
-      </c>
-      <c r="G71" s="103">
+        <v>208</v>
+      </c>
+      <c r="C71" s="90">
+        <v>1</v>
+      </c>
+      <c r="D71" s="91">
+        <v>1</v>
+      </c>
+      <c r="E71" s="91"/>
+      <c r="F71" s="92">
+        <v>1</v>
+      </c>
+      <c r="G71" s="92">
         <v>1</v>
       </c>
     </row>
@@ -3817,8 +3835,8 @@
       <c r="D77">
         <v>1</v>
       </c>
-      <c r="G77" s="2">
-        <v>1</v>
+      <c r="G77" s="92">
+        <v>2</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>13</v>
@@ -3922,8 +3940,8 @@
       <c r="D83">
         <v>2</v>
       </c>
-      <c r="G83" s="2">
-        <v>1</v>
+      <c r="G83" s="92">
+        <v>2</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>13</v>
@@ -3939,8 +3957,8 @@
       <c r="D84">
         <v>2</v>
       </c>
-      <c r="G84" s="2">
-        <v>1</v>
+      <c r="G84" s="92">
+        <v>2</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>13</v>
@@ -4095,8 +4113,8 @@
       <c r="D93">
         <v>1</v>
       </c>
-      <c r="G93" s="2">
-        <v>1</v>
+      <c r="G93" s="92">
+        <v>2</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>13</v>
@@ -4124,8 +4142,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4143,20 +4161,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
       <c r="F2" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="92"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
@@ -4220,7 +4238,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I6" s="10">
         <v>1</v>
@@ -4252,7 +4270,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I7" s="10">
         <v>0</v>
@@ -4284,16 +4302,16 @@
         <v>0</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I8" s="10">
         <v>1</v>
       </c>
-      <c r="J8" s="90" t="s">
+      <c r="J8" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -4318,16 +4336,16 @@
         <v>1</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I9" s="10">
         <v>1</v>
       </c>
-      <c r="J9" s="90" t="s">
+      <c r="J9" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4352,16 +4370,16 @@
         <v>0</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I10" s="10">
         <v>0</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="90"/>
-      <c r="L10" s="90"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -4386,16 +4404,16 @@
         <v>1</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I11" s="10">
         <v>0</v>
       </c>
-      <c r="J11" s="90" t="s">
+      <c r="J11" s="97" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -4420,16 +4438,16 @@
         <v>1</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I12" s="10">
         <v>1</v>
       </c>
-      <c r="J12" s="90" t="s">
+      <c r="J12" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
+      <c r="K12" s="97"/>
+      <c r="L12" s="97"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -4459,11 +4477,11 @@
       <c r="I13" s="10">
         <v>0</v>
       </c>
-      <c r="J13" s="90" t="s">
+      <c r="J13" s="97" t="s">
         <v>84</v>
       </c>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -4488,16 +4506,16 @@
         <v>1</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I14" s="10">
         <v>0</v>
       </c>
-      <c r="J14" s="90" t="s">
+      <c r="J14" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="97"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -4522,16 +4540,16 @@
         <v>1</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I15" s="10">
         <v>0</v>
       </c>
-      <c r="J15" s="90" t="s">
+      <c r="J15" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -4614,7 +4632,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I18" s="10">
         <v>1</v>
@@ -4680,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I20" s="10">
         <v>0</v>
@@ -4713,7 +4731,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I21" s="10">
         <v>1</v>
@@ -4742,7 +4760,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I22" s="10">
         <v>0</v>
@@ -4829,7 +4847,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I25" s="10">
         <v>0</v>
@@ -4858,7 +4876,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I26" s="10">
         <v>1</v>
@@ -4887,7 +4905,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="31" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I27" s="10">
         <v>1</v>
@@ -4916,7 +4934,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I28" s="10">
         <v>0</v>
@@ -4945,7 +4963,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I29" s="10">
         <v>1</v>
@@ -4974,7 +4992,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I30" s="10">
         <v>1</v>
@@ -5004,7 +5022,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I31" s="10">
         <v>1</v>
@@ -5034,7 +5052,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="31" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I32" s="10">
         <v>0</v>
@@ -5064,7 +5082,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I33" s="10">
         <v>1</v>
@@ -5124,7 +5142,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I35" s="10">
         <v>0</v>
@@ -5154,7 +5172,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I36" s="10">
         <v>0</v>
@@ -5174,7 +5192,7 @@
       <c r="D37" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="100">
+      <c r="E37" s="89">
         <v>26</v>
       </c>
       <c r="F37" s="21">
@@ -5204,7 +5222,7 @@
       <c r="D38" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="100">
+      <c r="E38" s="89">
         <v>26</v>
       </c>
       <c r="F38" s="36">
@@ -5214,7 +5232,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="M38" s="32"/>
     </row>
@@ -5231,7 +5249,7 @@
       <c r="D39" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="100">
+      <c r="E39" s="89">
         <v>26</v>
       </c>
       <c r="F39" s="36">
@@ -5258,7 +5276,7 @@
       <c r="D40" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="E40" s="100">
+      <c r="E40" s="89">
         <v>26</v>
       </c>
       <c r="F40" s="36">
@@ -5282,7 +5300,7 @@
       <c r="D41" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="E41" s="100">
+      <c r="E41" s="89">
         <v>26</v>
       </c>
       <c r="F41" s="36">
@@ -5309,8 +5327,8 @@
       <c r="D42" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="E42" s="104">
-        <v>10</v>
+      <c r="E42" s="93">
+        <v>14</v>
       </c>
       <c r="F42" s="36">
         <v>0</v>
@@ -5648,8 +5666,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:AMJ44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E29" sqref="E28:E29"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5665,13 +5683,13 @@
         <v>184</v>
       </c>
       <c r="B2" s="49"/>
-      <c r="F2" s="95" t="s">
+      <c r="F2" s="102" t="s">
         <v>185</v>
       </c>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5682,32 +5700,32 @@
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="103" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="103" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="101" t="s">
         <v>180</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="103" t="s">
         <v>181</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="101" t="s">
         <v>182</v>
       </c>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="99" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:1024" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="92"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="99"/>
       <c r="AMF5"/>
       <c r="AMG5"/>
       <c r="AMH5"/>
@@ -5898,10 +5916,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="97" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="90"/>
+      <c r="B17" s="97"/>
       <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5915,32 +5933,32 @@
       <c r="F18" s="57"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="92" t="s">
+      <c r="A19" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C19" s="92" t="s">
+      <c r="C19" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D19" s="94" t="s">
+      <c r="D19" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E19" s="92" t="s">
+      <c r="E19" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F19" s="94" t="s">
+      <c r="F19" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="94"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="94"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="101"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="51">
@@ -6136,36 +6154,36 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="92" t="s">
+      <c r="A34" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="B34" s="94" t="s">
+      <c r="B34" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C34" s="92" t="s">
+      <c r="C34" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D34" s="94" t="s">
+      <c r="D34" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E34" s="92" t="s">
+      <c r="E34" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F34" s="94" t="s">
+      <c r="F34" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="92"/>
-      <c r="B35" s="94"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="94"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
+      <c r="A35" s="99"/>
+      <c r="B35" s="101"/>
+      <c r="C35" s="99"/>
+      <c r="D35" s="101"/>
+      <c r="E35" s="99"/>
+      <c r="F35" s="101"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="51">
@@ -6625,7 +6643,7 @@
   <dimension ref="A3:B12"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6716,7 +6734,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A3:F145"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="D32" sqref="D29:D32"/>
     </sheetView>
   </sheetViews>
@@ -6728,32 +6746,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F3" s="94" t="s">
+      <c r="F3" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="98"/>
-      <c r="B4" s="94"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="94"/>
+      <c r="A4" s="105"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="101"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="51">
@@ -6846,32 +6864,32 @@
       <c r="F13" s="52"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="98" t="s">
+      <c r="A15" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="92" t="s">
+      <c r="C15" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="94" t="s">
+      <c r="D15" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E15" s="92" t="s">
+      <c r="E15" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F15" s="94" t="s">
+      <c r="F15" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="98"/>
-      <c r="B16" s="94"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="94"/>
+      <c r="A16" s="105"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="101"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="51">
@@ -6964,32 +6982,32 @@
       <c r="F25" s="52"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="98" t="s">
+      <c r="A27" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="92" t="s">
+      <c r="C27" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D27" s="94" t="s">
+      <c r="D27" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E27" s="92" t="s">
+      <c r="E27" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F27" s="94" t="s">
+      <c r="F27" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="98"/>
-      <c r="B28" s="94"/>
-      <c r="C28" s="92"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="92"/>
-      <c r="F28" s="94"/>
+      <c r="A28" s="105"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="101"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="51">
@@ -7082,32 +7100,32 @@
       <c r="F37" s="52"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="98" t="s">
+      <c r="A39" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="94" t="s">
+      <c r="B39" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C39" s="92" t="s">
+      <c r="C39" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D39" s="94" t="s">
+      <c r="D39" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E39" s="92" t="s">
+      <c r="E39" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F39" s="94" t="s">
+      <c r="F39" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="98"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="92"/>
-      <c r="D40" s="94"/>
-      <c r="E40" s="92"/>
-      <c r="F40" s="94"/>
+      <c r="A40" s="105"/>
+      <c r="B40" s="101"/>
+      <c r="C40" s="99"/>
+      <c r="D40" s="101"/>
+      <c r="E40" s="99"/>
+      <c r="F40" s="101"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="51">
@@ -7200,32 +7218,32 @@
       <c r="F49" s="52"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="98" t="s">
+      <c r="A51" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="94" t="s">
+      <c r="B51" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C51" s="92" t="s">
+      <c r="C51" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D51" s="94" t="s">
+      <c r="D51" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E51" s="92" t="s">
+      <c r="E51" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F51" s="94" t="s">
+      <c r="F51" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="98"/>
-      <c r="B52" s="94"/>
-      <c r="C52" s="92"/>
-      <c r="D52" s="94"/>
-      <c r="E52" s="92"/>
-      <c r="F52" s="94"/>
+      <c r="A52" s="105"/>
+      <c r="B52" s="101"/>
+      <c r="C52" s="99"/>
+      <c r="D52" s="101"/>
+      <c r="E52" s="99"/>
+      <c r="F52" s="101"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="51">
@@ -7318,32 +7336,32 @@
       <c r="F61" s="52"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="98" t="s">
+      <c r="A63" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="94" t="s">
+      <c r="B63" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C63" s="92" t="s">
+      <c r="C63" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D63" s="94" t="s">
+      <c r="D63" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E63" s="92" t="s">
+      <c r="E63" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F63" s="94" t="s">
+      <c r="F63" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="98"/>
-      <c r="B64" s="94"/>
-      <c r="C64" s="92"/>
-      <c r="D64" s="94"/>
-      <c r="E64" s="92"/>
-      <c r="F64" s="94"/>
+      <c r="A64" s="105"/>
+      <c r="B64" s="101"/>
+      <c r="C64" s="99"/>
+      <c r="D64" s="101"/>
+      <c r="E64" s="99"/>
+      <c r="F64" s="101"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="51">
@@ -7436,32 +7454,32 @@
       <c r="F73" s="52"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="98" t="s">
+      <c r="A75" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B75" s="94" t="s">
+      <c r="B75" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C75" s="92" t="s">
+      <c r="C75" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D75" s="94" t="s">
+      <c r="D75" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E75" s="92" t="s">
+      <c r="E75" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F75" s="94" t="s">
+      <c r="F75" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="98"/>
-      <c r="B76" s="94"/>
-      <c r="C76" s="92"/>
-      <c r="D76" s="94"/>
-      <c r="E76" s="92"/>
-      <c r="F76" s="94"/>
+      <c r="A76" s="105"/>
+      <c r="B76" s="101"/>
+      <c r="C76" s="99"/>
+      <c r="D76" s="101"/>
+      <c r="E76" s="99"/>
+      <c r="F76" s="101"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="51">
@@ -7554,32 +7572,32 @@
       <c r="F85" s="52"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="98" t="s">
+      <c r="A87" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="B87" s="94" t="s">
+      <c r="B87" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C87" s="92" t="s">
+      <c r="C87" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D87" s="94" t="s">
+      <c r="D87" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E87" s="92" t="s">
+      <c r="E87" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F87" s="94" t="s">
+      <c r="F87" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="98"/>
-      <c r="B88" s="94"/>
-      <c r="C88" s="92"/>
-      <c r="D88" s="94"/>
-      <c r="E88" s="92"/>
-      <c r="F88" s="94"/>
+      <c r="A88" s="105"/>
+      <c r="B88" s="101"/>
+      <c r="C88" s="99"/>
+      <c r="D88" s="101"/>
+      <c r="E88" s="99"/>
+      <c r="F88" s="101"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="51">
@@ -7680,32 +7698,32 @@
       <c r="F97" s="52"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="98">
-        <v>2</v>
-      </c>
-      <c r="B99" s="94" t="s">
+      <c r="A99" s="105">
+        <v>2</v>
+      </c>
+      <c r="B99" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C99" s="92" t="s">
+      <c r="C99" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D99" s="94" t="s">
+      <c r="D99" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E99" s="92" t="s">
+      <c r="E99" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F99" s="94" t="s">
+      <c r="F99" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="98"/>
-      <c r="B100" s="94"/>
-      <c r="C100" s="92"/>
-      <c r="D100" s="94"/>
-      <c r="E100" s="92"/>
-      <c r="F100" s="94"/>
+      <c r="A100" s="105"/>
+      <c r="B100" s="101"/>
+      <c r="C100" s="99"/>
+      <c r="D100" s="101"/>
+      <c r="E100" s="99"/>
+      <c r="F100" s="101"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="51">
@@ -7798,32 +7816,32 @@
       <c r="F109" s="52"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="98">
+      <c r="A111" s="105">
         <v>3</v>
       </c>
-      <c r="B111" s="94" t="s">
+      <c r="B111" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C111" s="92" t="s">
+      <c r="C111" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D111" s="94" t="s">
+      <c r="D111" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E111" s="92" t="s">
+      <c r="E111" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F111" s="94" t="s">
+      <c r="F111" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="98"/>
-      <c r="B112" s="94"/>
-      <c r="C112" s="92"/>
-      <c r="D112" s="94"/>
-      <c r="E112" s="92"/>
-      <c r="F112" s="94"/>
+      <c r="A112" s="105"/>
+      <c r="B112" s="101"/>
+      <c r="C112" s="99"/>
+      <c r="D112" s="101"/>
+      <c r="E112" s="99"/>
+      <c r="F112" s="101"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="51">
@@ -7916,32 +7934,32 @@
       <c r="F121" s="52"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="98" t="s">
+      <c r="A123" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="B123" s="94" t="s">
+      <c r="B123" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C123" s="92" t="s">
+      <c r="C123" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="D123" s="94" t="s">
+      <c r="D123" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E123" s="92" t="s">
+      <c r="E123" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="F123" s="94" t="s">
+      <c r="F123" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="98"/>
-      <c r="B124" s="94"/>
-      <c r="C124" s="92"/>
-      <c r="D124" s="94"/>
-      <c r="E124" s="92"/>
-      <c r="F124" s="94"/>
+      <c r="A124" s="105"/>
+      <c r="B124" s="101"/>
+      <c r="C124" s="99"/>
+      <c r="D124" s="101"/>
+      <c r="E124" s="99"/>
+      <c r="F124" s="101"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="51">
@@ -8042,32 +8060,32 @@
       <c r="F133" s="52"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="97">
+      <c r="A135" s="104">
         <v>4</v>
       </c>
-      <c r="B135" s="94" t="s">
+      <c r="B135" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C135" s="94" t="s">
+      <c r="C135" s="101" t="s">
         <v>180</v>
       </c>
-      <c r="D135" s="94" t="s">
+      <c r="D135" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E135" s="94" t="s">
+      <c r="E135" s="101" t="s">
         <v>182</v>
       </c>
-      <c r="F135" s="94" t="s">
+      <c r="F135" s="101" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="97"/>
-      <c r="B136" s="94"/>
-      <c r="C136" s="94"/>
-      <c r="D136" s="94"/>
-      <c r="E136" s="94"/>
-      <c r="F136" s="94"/>
+      <c r="A136" s="104"/>
+      <c r="B136" s="101"/>
+      <c r="C136" s="101"/>
+      <c r="D136" s="101"/>
+      <c r="E136" s="101"/>
+      <c r="F136" s="101"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="51">
@@ -8249,7 +8267,7 @@
   <dimension ref="A2:P12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8265,43 +8283,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="106" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="101" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="94" t="s">
+      <c r="D2" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="E2" s="94" t="s">
+      <c r="E2" s="101" t="s">
         <v>182</v>
       </c>
-      <c r="F2" s="94" t="s">
+      <c r="F2" s="101" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="95" t="s">
+      <c r="H2" s="102" t="s">
         <v>199</v>
       </c>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
+      <c r="A3" s="106"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="51">
@@ -8314,7 +8332,7 @@
         <v>201</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>203</v>
@@ -8334,7 +8352,7 @@
         <v>201</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>203</v>
@@ -8432,8 +8450,8 @@
       <c r="D10" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="E10" s="51" t="s">
-        <v>207</v>
+      <c r="E10" s="94" t="s">
+        <v>217</v>
       </c>
       <c r="F10" s="52"/>
     </row>
@@ -8450,8 +8468,8 @@
       <c r="D11" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>208</v>
+      <c r="E11" s="95" t="s">
+        <v>207</v>
       </c>
       <c r="F11" s="15"/>
     </row>
@@ -8468,8 +8486,8 @@
       <c r="D12" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="E12" s="51" t="s">
-        <v>208</v>
+      <c r="E12" s="94" t="s">
+        <v>207</v>
       </c>
       <c r="F12" s="52"/>
     </row>

</xml_diff>